<commit_message>
insert data to table
</commit_message>
<xml_diff>
--- a/qc/static/qc/QC Seiscomp.xlsx
+++ b/qc/static/qc/QC Seiscomp.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>QUALITY CONTROL (QC-3)</t>
   </si>
@@ -98,100 +98,10 @@
     <t>Ket</t>
   </si>
   <si>
-    <t>11.89771 S</t>
-  </si>
-  <si>
-    <t>166.39536 E</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>10 km</t>
-  </si>
-  <si>
-    <t>Santa Cruz Islands</t>
-  </si>
-  <si>
     <t>Prev</t>
   </si>
   <si>
-    <t>12.15061 S</t>
-  </si>
-  <si>
-    <t>165.96417 E</t>
-  </si>
-  <si>
-    <t>mb</t>
-  </si>
-  <si>
-    <t>35 km</t>
-  </si>
-  <si>
     <t>QC</t>
-  </si>
-  <si>
-    <t>4.62873 S</t>
-  </si>
-  <si>
-    <t>130.26984 E</t>
-  </si>
-  <si>
-    <t>11 km</t>
-  </si>
-  <si>
-    <t>Banda Sea</t>
-  </si>
-  <si>
-    <t>4.71038 S</t>
-  </si>
-  <si>
-    <t>130.24854 E</t>
-  </si>
-  <si>
-    <t>MLv</t>
-  </si>
-  <si>
-    <t>18 km</t>
-  </si>
-  <si>
-    <t>7.01574 S</t>
-  </si>
-  <si>
-    <t>129.64021 E</t>
-  </si>
-  <si>
-    <t>176 km</t>
-  </si>
-  <si>
-    <t>6.72474 S</t>
-  </si>
-  <si>
-    <t>129.48380 E</t>
-  </si>
-  <si>
-    <t>130 km</t>
-  </si>
-  <si>
-    <t>8.20744 S</t>
-  </si>
-  <si>
-    <t>119.79731 E</t>
-  </si>
-  <si>
-    <t>171 km</t>
-  </si>
-  <si>
-    <t>Flores Region, Indonesia</t>
-  </si>
-  <si>
-    <t>8.18256 S</t>
-  </si>
-  <si>
-    <t>119.83324 E</t>
-  </si>
-  <si>
-    <t>174 km</t>
   </si>
   <si>
     <t xml:space="preserve">Mengetahui, </t>
@@ -1509,10 +1419,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N998"/>
+  <dimension ref="B1:N992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -1659,327 +1569,141 @@
       <c r="B8" s="11">
         <v>1</v>
       </c>
-      <c r="C8" s="12">
-        <v>45637</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.697199074074074</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="14" t="s">
+    </row>
+    <row r="9" ht="18" customHeight="1" spans="2:14">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="14">
-        <v>5.46</v>
-      </c>
-      <c r="H8" s="14" t="s">
+    </row>
+    <row r="10" ht="14.4" customHeight="1" spans="2:14">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" ht="14.4" customHeight="1" spans="2:14">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" ht="23.4" customHeight="1" spans="2:14">
+      <c r="B12" s="19"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="E12" s="22"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="14">
-        <v>90</v>
-      </c>
-      <c r="K8" s="14">
-        <v>1</v>
-      </c>
-      <c r="L8" s="14">
-        <v>168</v>
-      </c>
-      <c r="M8" s="32" t="s">
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" spans="2:14">
+      <c r="B13" s="19"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="E13" s="23"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" ht="18" customHeight="1" spans="2:14">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16">
-        <v>45637</v>
-      </c>
-      <c r="D9" s="17">
-        <v>0.697280092592593</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="18">
-        <v>5.42</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="18">
-        <v>105</v>
-      </c>
-      <c r="K9" s="18">
-        <v>2</v>
-      </c>
-      <c r="L9" s="18">
-        <v>84</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" ht="18" customHeight="1" spans="2:14">
-      <c r="B10" s="11">
-        <v>2</v>
-      </c>
-      <c r="C10" s="12">
-        <v>45637</v>
-      </c>
-      <c r="D10" s="13">
-        <v>0.75849537037037</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="14">
-        <v>3.76</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="14">
-        <v>28</v>
-      </c>
-      <c r="K10" s="14">
-        <v>1</v>
-      </c>
-      <c r="L10" s="14">
-        <v>173</v>
-      </c>
-      <c r="M10" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" ht="18" customHeight="1" spans="2:14">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16">
-        <v>45637</v>
-      </c>
-      <c r="D11" s="17">
-        <v>0.75849537037037</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="18">
-        <v>3.84</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="18">
-        <v>47</v>
-      </c>
-      <c r="K11" s="18">
-        <v>1.6</v>
-      </c>
-      <c r="L11" s="18">
-        <v>134</v>
-      </c>
-      <c r="M11" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" ht="18" customHeight="1" spans="2:14">
-      <c r="B12" s="11">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12">
-        <v>45637</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0.774780092592593</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="14">
-        <v>4.37</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="14">
-        <v>20</v>
-      </c>
-      <c r="K12" s="14">
-        <v>1</v>
-      </c>
-      <c r="L12" s="14">
-        <v>83</v>
-      </c>
-      <c r="M12" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" ht="18" customHeight="1" spans="2:14">
-      <c r="B13" s="15"/>
-      <c r="C13" s="16">
-        <v>45637</v>
-      </c>
-      <c r="D13" s="17">
-        <v>0.774780092592593</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="18">
-        <v>4.47</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="18">
-        <v>42</v>
-      </c>
-      <c r="K13" s="18">
-        <v>2</v>
-      </c>
-      <c r="L13" s="18">
-        <v>109</v>
-      </c>
-      <c r="M13" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" ht="18" customHeight="1" spans="2:14">
-      <c r="B14" s="11">
-        <v>4</v>
-      </c>
-      <c r="C14" s="12">
-        <v>45637</v>
-      </c>
-      <c r="D14" s="13">
-        <v>0.783171296296296</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="14">
-        <v>3.59</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="14">
-        <v>48</v>
-      </c>
-      <c r="K14" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="L14" s="14">
-        <v>93</v>
-      </c>
-      <c r="M14" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" ht="18" customHeight="1" spans="2:14">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16">
-        <v>45637</v>
-      </c>
-      <c r="D15" s="17">
-        <v>0.783159722222222</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="18">
-        <v>3.66</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="18">
-        <v>76</v>
-      </c>
-      <c r="K15" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="L15" s="18">
-        <v>90</v>
-      </c>
-      <c r="M15" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" ht="14.4" customHeight="1" spans="2:14">
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" spans="2:14">
+      <c r="B14" s="19"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" spans="2:14">
+      <c r="B15" s="19"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="19"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" spans="2:14">
       <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="19"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
@@ -1987,14 +1711,14 @@
       <c r="J16" s="19"/>
       <c r="K16" s="20"/>
       <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
+      <c r="M16" s="26"/>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" ht="14.4" customHeight="1" spans="2:14">
+    <row r="17" ht="15.75" customHeight="1" spans="2:14">
       <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="19"/>
       <c r="G17" s="20"/>
       <c r="H17" s="21"/>
@@ -2002,16 +1726,16 @@
       <c r="J17" s="19"/>
       <c r="K17" s="20"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
+      <c r="M17" s="26"/>
       <c r="N17" s="19"/>
     </row>
-    <row r="18" ht="23.4" customHeight="1" spans="2:14">
+    <row r="18" ht="15.75" customHeight="1" spans="2:14">
       <c r="B18" s="19"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23" t="s">
-        <v>55</v>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27" t="s">
+        <v>29</v>
       </c>
-      <c r="E18" s="22"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="19"/>
       <c r="G18" s="20"/>
       <c r="H18" s="21"/>
@@ -2019,18 +1743,18 @@
       <c r="J18" s="19"/>
       <c r="K18" s="20"/>
       <c r="L18" s="19"/>
-      <c r="M18" s="23" t="s">
-        <v>56</v>
+      <c r="M18" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="N18" s="19"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" spans="2:14">
       <c r="B19" s="19"/>
-      <c r="C19" s="24"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="25" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
-      <c r="E19" s="23"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="19"/>
       <c r="G19" s="20"/>
       <c r="H19" s="21"/>
@@ -2038,114 +1762,46 @@
       <c r="J19" s="19"/>
       <c r="K19" s="20"/>
       <c r="L19" s="19"/>
-      <c r="M19" s="23" t="s">
-        <v>58</v>
+      <c r="M19" s="29" t="s">
+        <v>32</v>
       </c>
       <c r="N19" s="19"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1" spans="2:14">
-      <c r="B20" s="19"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="19"/>
+    <row r="20" ht="15.75" customHeight="1" spans="7:13">
       <c r="G20" s="20"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
       <c r="K20" s="20"/>
-      <c r="L20" s="19"/>
       <c r="M20" s="26"/>
-      <c r="N20" s="19"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" spans="2:14">
-      <c r="B21" s="19"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="19"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" spans="7:11">
       <c r="G21" s="20"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
       <c r="K21" s="20"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="19"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" spans="2:14">
-      <c r="B22" s="19"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="19"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" spans="7:11">
       <c r="G22" s="20"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
       <c r="K22" s="20"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="19"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1" spans="2:14">
-      <c r="B23" s="19"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="19"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" spans="7:11">
       <c r="G23" s="20"/>
       <c r="H23" s="21"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
       <c r="K23" s="20"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="19"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1" spans="2:14">
-      <c r="B24" s="19"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="19"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" spans="7:11">
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
       <c r="K24" s="20"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="N24" s="19"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1" spans="2:14">
-      <c r="B25" s="19"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="19"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" spans="7:11">
       <c r="G25" s="20"/>
       <c r="H25" s="21"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
       <c r="K25" s="20"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="N25" s="19"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" spans="7:13">
+    </row>
+    <row r="26" ht="15.75" customHeight="1" spans="7:11">
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
       <c r="K26" s="20"/>
-      <c r="M26" s="26"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="7:11">
       <c r="G27" s="20"/>
@@ -6977,38 +6633,8 @@
       <c r="H992" s="21"/>
       <c r="K992" s="20"/>
     </row>
-    <row r="993" ht="15.75" customHeight="1" spans="7:11">
-      <c r="G993" s="20"/>
-      <c r="H993" s="21"/>
-      <c r="K993" s="20"/>
-    </row>
-    <row r="994" ht="15.75" customHeight="1" spans="7:11">
-      <c r="G994" s="20"/>
-      <c r="H994" s="21"/>
-      <c r="K994" s="20"/>
-    </row>
-    <row r="995" ht="15.75" customHeight="1" spans="7:11">
-      <c r="G995" s="20"/>
-      <c r="H995" s="21"/>
-      <c r="K995" s="20"/>
-    </row>
-    <row r="996" ht="15.75" customHeight="1" spans="7:11">
-      <c r="G996" s="20"/>
-      <c r="H996" s="21"/>
-      <c r="K996" s="20"/>
-    </row>
-    <row r="997" ht="15.75" customHeight="1" spans="7:11">
-      <c r="G997" s="20"/>
-      <c r="H997" s="21"/>
-      <c r="K997" s="20"/>
-    </row>
-    <row r="998" ht="15.75" customHeight="1" spans="7:11">
-      <c r="G998" s="20"/>
-      <c r="H998" s="21"/>
-      <c r="K998" s="20"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="9">
     <mergeCell ref="B1:N1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
@@ -7018,9 +6644,6 @@
     <mergeCell ref="G6:K6"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait"/>

</xml_diff>

<commit_message>
Make the date, name and NIP to be dynamic based on the rows added
</commit_message>
<xml_diff>
--- a/qc/static/qc/QC Seiscomp.xlsx
+++ b/qc/static/qc/QC Seiscomp.xlsx
@@ -1366,7 +1366,7 @@
   <dimension ref="B1:N990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -1539,7 +1539,7 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" ht="23.4" customHeight="1" spans="2:14">
+    <row r="10" ht="23.4" spans="2:14">
       <c r="B10" s="10"/>
       <c r="C10" s="13"/>
       <c r="D10" s="14" t="s">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="2:14">
+    <row r="11" ht="23.4" spans="2:14">
       <c r="B11" s="10"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16" t="s">

</xml_diff>